<commit_message>
Cek Stok, Set onkir, change Column
</commit_message>
<xml_diff>
--- a/database/FileExcel/Barang.xlsx
+++ b/database/FileExcel/Barang.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yovie\persediaanapp-magang\database\FileExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3. Bahan Kerja\hosting\yovie\database\FileExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BB7EA8-EC14-4D0B-A9CB-A6062AA10A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A335A6-C8B8-4983-8915-08E5558128EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="2990" windowWidth="11440" windowHeight="7810" xr2:uid="{19905B0D-1A8A-4576-91B2-29E87108E41B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{19905B0D-1A8A-4576-91B2-29E87108E41B}"/>
   </bookViews>
   <sheets>
     <sheet name="barang" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>id</t>
   </si>
@@ -194,24 +194,22 @@
   </si>
   <si>
     <t>tas3.jpg</t>
+  </si>
+  <si>
+    <t>berat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri "/>
     </font>
     <font>
       <sz val="8"/>
@@ -240,9 +238,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,24 +557,24 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H21" activeCellId="1" sqref="H2:H11 H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" customWidth="1"/>
-    <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" customWidth="1"/>
-    <col min="7" max="7" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.7265625" customWidth="1"/>
-    <col min="10" max="11" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="139.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -600,22 +597,25 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -638,17 +638,19 @@
         <v>15</v>
       </c>
       <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -671,17 +673,19 @@
         <v>15</v>
       </c>
       <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -704,17 +708,19 @@
         <v>15</v>
       </c>
       <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
         <v>11</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -737,17 +743,19 @@
         <v>15</v>
       </c>
       <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
         <v>11</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>47</v>
       </c>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -770,17 +778,19 @@
         <v>15</v>
       </c>
       <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
         <v>11</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>51</v>
       </c>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -803,16 +813,19 @@
         <v>15</v>
       </c>
       <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
         <v>11</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -835,16 +848,19 @@
         <v>15</v>
       </c>
       <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
         <v>11</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -867,16 +883,19 @@
         <v>15</v>
       </c>
       <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
         <v>11</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -899,16 +918,19 @@
         <v>15</v>
       </c>
       <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
         <v>11</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -931,17 +953,20 @@
         <v>15</v>
       </c>
       <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
         <v>11</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>